<commit_message>
sort alternate source field columns
</commit_message>
<xml_diff>
--- a/tests/011_AlternateSourceFields.xlsx
+++ b/tests/011_AlternateSourceFields.xlsx
@@ -50,22 +50,22 @@
     <t xml:space="preserve">str2date</t>
   </si>
   <si>
+    <t xml:space="preserve">Alternate Source Field 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alternate Source Field 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Alternate Source Field 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sex</t>
   </si>
   <si>
     <t xml:space="preserve">gender</t>
   </si>
   <si>
+    <t xml:space="preserve">sex0</t>
+  </si>
+  <si>
     <t xml:space="preserve">sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sex0</t>
   </si>
 </sst>
 </file>
@@ -181,11 +181,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5446428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0892857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1294642857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1607142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.3392857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1919642857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8526785714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7723214285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8035714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.8705357142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,16 +245,17 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5446428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0892857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1294642857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1607142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.3392857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1919642857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8526785714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7723214285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.8705357142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8035714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,7 +309,7 @@
     <oddFooter/>
   </headerFooter>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="6" man="true" max="65535" min="0"/>
+    <brk id="5" man="true" max="65535" min="0"/>
   </colBreaks>
 </worksheet>
 </file>
</xml_diff>